<commit_message>
Start calculation loop and stopwatch after pressing enter, update result spreadsheet
</commit_message>
<xml_diff>
--- a/doc/calculations_per_minute.xlsx
+++ b/doc/calculations_per_minute.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michi\git\math-trainer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D210B3E8-9F3B-4E0A-B188-15B047141B91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5202CB-A21D-4B34-BE79-BA4A2A370D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{892C049C-B713-466F-A042-A488F99F1905}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Michi</t>
   </si>
@@ -54,6 +54,34 @@
   </si>
   <si>
     <t>errors</t>
+  </si>
+  <si>
+    <t>Nani</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Timo</t>
+  </si>
+  <si>
+    <t>NUR 1x1:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michi </t>
+  </si>
+  <si>
+    <t>ALLE RECHNUNGEN
+von 30 auf 20 reduzieren</t>
+  </si>
+  <si>
+    <t>(30 ist ok)</t>
+  </si>
+  <si>
+    <t>Neni</t>
+  </si>
+  <si>
+    <t>24,34</t>
   </si>
 </sst>
 </file>
@@ -69,12 +97,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -102,6 +142,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,34 +464,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7277625-5EA1-4E03-86A8-09C9CAB89A71}">
-  <dimension ref="C6:M13"/>
+  <dimension ref="C5:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
       <c r="D6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
       <c r="D7" s="2" t="s">
         <v>1</v>
@@ -458,8 +535,9 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
@@ -467,16 +545,21 @@
         <v>100</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="2">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
@@ -484,16 +567,21 @@
         <v>100</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="2">
+        <v>100</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
@@ -501,16 +589,21 @@
         <v>10</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2">
+        <v>10</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="3:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
@@ -518,16 +611,31 @@
         <v>13</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="F11" s="2">
+        <v>16</v>
+      </c>
+      <c r="G11" s="2">
+        <v>19</v>
+      </c>
+      <c r="H11" s="2">
+        <v>4</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="2">
+        <v>25</v>
+      </c>
+      <c r="K11" s="2">
+        <v>11</v>
+      </c>
+      <c r="L11" s="2">
+        <v>22</v>
+      </c>
       <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" s="4" t="s">
         <v>6</v>
       </c>
@@ -535,16 +643,31 @@
         <v>1</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3</v>
+      </c>
+      <c r="H12" s="2">
+        <v>11</v>
+      </c>
+      <c r="I12" s="2">
+        <v>3</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>3</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
       <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -556,8 +679,12 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F5:H5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>